<commit_message>
add utilities to reactor objects
</commit_message>
<xml_diff>
--- a/excel files/data_propionibacteria.xlsx
+++ b/excel files/data_propionibacteria.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Reboots\PycharmProjects\Alquimia\excel files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38BD6124-B14D-4957-987C-87DC42F74D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5954DE16-4793-42AF-BA9D-740F772AE7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="1845" windowWidth="20730" windowHeight="11160" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="1" r:id="rId1"/>
@@ -163,15 +163,6 @@
     <t>ace == glu*0.0021470197960763663+pH*0.010062441241181396, prop == glu*0.0008586272965669681+pH*0.00128523604994718, but == glu*0.00343240244820466+pH*-0.007526404480666873</t>
   </si>
   <si>
-    <t xml:space="preserve">utility bounds </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pH </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5,8 </t>
-  </si>
-  <si>
     <t>ace, prop, but</t>
   </si>
   <si>
@@ -188,6 +179,15 @@
   </si>
   <si>
     <t>prop == 0.235119469454648 * glu</t>
+  </si>
+  <si>
+    <t>utility_bounds</t>
+  </si>
+  <si>
+    <t>[5,8] ; [50,100]</t>
+  </si>
+  <si>
+    <t>pH ; energy</t>
   </si>
 </sst>
 </file>
@@ -669,7 +669,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -971,22 +971,22 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1038,7 +1038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1064,7 +1064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1090,7 +1090,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1116,7 +1116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1168,7 +1168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1194,7 +1194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>3</v>
       </c>
@@ -1220,7 +1220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>3</v>
       </c>
@@ -1246,7 +1246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1288,24 +1288,24 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.08984375" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1328,7 +1328,7 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -1337,7 +1337,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>24</v>
       </c>
@@ -1351,7 +1351,7 @@
         <v>38</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="F2">
         <v>0.26675654674413302</v>
@@ -1369,7 +1369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1383,7 +1383,7 @@
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F3">
         <v>0.28253562825913597</v>
@@ -1401,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F4">
         <v>0.26792861197630802</v>
@@ -1433,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -1447,7 +1447,7 @@
         <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="F5">
         <v>0.376575631424244</v>
@@ -1465,7 +1465,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>27</v>
       </c>
@@ -1479,7 +1479,7 @@
         <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F6">
         <v>0.23511946945464801</v>
@@ -1497,7 +1497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1508,7 +1508,7 @@
         <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E7" t="s">
         <v>40</v>
@@ -1517,10 +1517,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="I7">
         <v>0</v>
@@ -1547,21 +1547,21 @@
       <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="13" max="13" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1596,7 +1596,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>24</v>
       </c>
@@ -1666,7 +1666,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1769,7 +1769,7 @@
       </c>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -1839,7 +1839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1874,7 +1874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1990,18 +1990,18 @@
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -2027,7 +2027,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2053,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2079,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2150,24 +2150,24 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="5"/>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>13</v>
       </c>
@@ -2175,7 +2175,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="6" t="s">
         <v>15</v>
       </c>
@@ -2183,7 +2183,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>16</v>
       </c>
@@ -2191,37 +2191,37 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="2"/>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B9" s="7"/>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>16</v>
       </c>
       <c r="B10" s="9"/>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="B12" s="5"/>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>19</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" s="6" t="s">
         <v>20</v>
       </c>
@@ -2237,7 +2237,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>16</v>
       </c>

</xml_diff>

<commit_message>
working version of making input/reactor intervals objects
</commit_message>
<xml_diff>
--- a/excel files/data_propionibacteria.xlsx
+++ b/excel files/data_propionibacteria.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5954DE16-4793-42AF-BA9D-740F772AE7B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC171356-7E1B-4673-8693-ED9C455102BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" activeTab="1" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="1560" yWindow="890" windowWidth="14840" windowHeight="9090" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
   <si>
     <t>components</t>
   </si>
@@ -142,9 +142,6 @@
     <t xml:space="preserve">glu </t>
   </si>
   <si>
-    <t xml:space="preserve">inputs </t>
-  </si>
-  <si>
     <t>glu</t>
   </si>
   <si>
@@ -188,6 +185,15 @@
   </si>
   <si>
     <t>pH ; energy</t>
+  </si>
+  <si>
+    <t>inputs</t>
+  </si>
+  <si>
+    <t>ace</t>
+  </si>
+  <si>
+    <t>but</t>
   </si>
 </sst>
 </file>
@@ -965,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1032,7 +1038,7 @@
         <v>0</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1213,11 +1219,11 @@
       <c r="F9">
         <v>1</v>
       </c>
-      <c r="G9">
-        <v>0</v>
+      <c r="G9" s="13" t="s">
+        <v>50</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1239,11 +1245,11 @@
       <c r="F10">
         <v>2</v>
       </c>
-      <c r="G10">
-        <v>0</v>
+      <c r="G10" s="13" t="s">
+        <v>37</v>
       </c>
       <c r="H10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1265,12 +1271,15 @@
       <c r="F11">
         <v>3</v>
       </c>
-      <c r="G11">
-        <v>0</v>
+      <c r="G11" s="13" t="s">
+        <v>51</v>
       </c>
       <c r="H11">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G12" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -1287,8 +1296,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE2DC50F-7E38-4E45-9660-C41E1DA6142A}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1313,22 +1322,22 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>34</v>
+        <v>49</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
@@ -1345,13 +1354,13 @@
         <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F2">
         <v>0.26675654674413302</v>
@@ -1377,13 +1386,13 @@
         <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F3">
         <v>0.28253562825913597</v>
@@ -1409,13 +1418,13 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4">
         <v>0.26792861197630802</v>
@@ -1441,13 +1450,13 @@
         <v>26</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F5">
         <v>0.376575631424244</v>
@@ -1473,13 +1482,13 @@
         <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6">
         <v>0.23511946945464801</v>
@@ -1505,22 +1514,22 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F7" s="13">
         <v>0</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I7">
         <v>0</v>

</xml_diff>

<commit_message>
added sum of products to output constraints
</commit_message>
<xml_diff>
--- a/excel files/data_propionibacteria.xlsx
+++ b/excel files/data_propionibacteria.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC171356-7E1B-4673-8693-ED9C455102BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71F69E00-331B-4778-BF8F-F9AAE075362C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="890" windowWidth="14840" windowHeight="9090" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
+    <workbookView xWindow="1560" yWindow="890" windowWidth="14840" windowHeight="9090" tabRatio="683" activeTab="2" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
     <sheet name="components" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="56">
   <si>
     <t>components</t>
   </si>
@@ -194,6 +194,18 @@
   </si>
   <si>
     <t>but</t>
+  </si>
+  <si>
+    <t>input_glucose</t>
+  </si>
+  <si>
+    <t>acetate</t>
+  </si>
+  <si>
+    <t>propionate</t>
+  </si>
+  <si>
+    <t>buytrate</t>
   </si>
 </sst>
 </file>
@@ -502,7 +514,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t> at which streams connect to the reactors (i.e wat are the reactor inputs and how are they connected)</a:t>
+            <a:t> at which streams connect to the next intervall (i.e wat are the reactor inputs and how are they connected to their outputs)</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -973,8 +985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54AE4236-3006-4E07-A9E2-DEE610CD0DBE}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1023,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -1297,7 +1309,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1552,13 +1564,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.36328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.26953125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" bestFit="1" customWidth="1"/>
@@ -1575,7 +1588,7 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s">
         <v>24</v>
@@ -1596,18 +1609,18 @@
         <v>32</v>
       </c>
       <c r="I1" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="J1" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="K1" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
Nov 2, major changes to superstructure generation
</commit_message>
<xml_diff>
--- a/excel files/data_propionibacteria.xlsx
+++ b/excel files/data_propionibacteria.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lucas\PycharmProjects\Alquimia\excel files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F33041E-7085-49F6-8E06-29BF48F04131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4170E7D3-963D-4059-B08B-E3F467BF1A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="683" xr2:uid="{6BCA81A1-C24E-4458-B51D-F7D92A8A2CBE}"/>
   </bookViews>
   <sheets>
-    <sheet name="components" sheetId="1" r:id="rId1"/>
-    <sheet name="reactors" sheetId="2" r:id="rId2"/>
-    <sheet name="connectionMatrix" sheetId="11" r:id="rId3"/>
+    <sheet name="Intervals" sheetId="1" r:id="rId1"/>
+    <sheet name="Reactors" sheetId="2" r:id="rId2"/>
+    <sheet name="ConnectionMatrix" sheetId="11" r:id="rId3"/>
     <sheet name="input_output" sheetId="13" r:id="rId4"/>
     <sheet name="eg reactor sheet" sheetId="12" r:id="rId5"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="70">
   <si>
     <t>components</t>
   </si>
@@ -157,9 +157,6 @@
     <t>conversion_factor</t>
   </si>
   <si>
-    <t>ace == glu*0.0021470197960763663+pH*0.010062441241181396, prop == glu*0.0008586272965669681+pH*0.00128523604994718, but == glu*0.00343240244820466+pH*-0.007526404480666873</t>
-  </si>
-  <si>
     <t>ace, prop, but</t>
   </si>
   <si>
@@ -220,16 +217,37 @@
     <t>seperation_coef</t>
   </si>
   <si>
-    <t>[1,0]</t>
-  </si>
-  <si>
-    <t>[1,0,0]; [0,1,0]</t>
-  </si>
-  <si>
-    <t>reject</t>
-  </si>
-  <si>
-    <t>permeate</t>
+    <t>[1,0,0]; [0,1,0]; [0,0,1]</t>
+  </si>
+  <si>
+    <t>[1,0];[0,1]</t>
+  </si>
+  <si>
+    <t>sep1</t>
+  </si>
+  <si>
+    <t>sep2</t>
+  </si>
+  <si>
+    <t>sep3</t>
+  </si>
+  <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>prot</t>
+  </si>
+  <si>
+    <t>glu, prot</t>
+  </si>
+  <si>
+    <t>ace == glu*0.0021470197960763663+pH*0.010062441241181396+ 0.2*prot , prop == glu*0.0008586272965669681+pH*0.00128523604994718+0.2*prot, but == glu*0.00343240244820466+pH*-0.007526404480666873 + 0.02*prot</t>
+  </si>
+  <si>
+    <t>bool , mix</t>
+  </si>
+  <si>
+    <t>mix</t>
   </si>
 </sst>
 </file>
@@ -442,7 +460,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -497,23 +515,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>257175</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>123823</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>768350</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>793750</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="TextBox 1">
+        <xdr:cNvPr id="2" name="CuadroTexto 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2166CD1C-89AD-4CD0-85A6-EA82146B47E2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E61CD0C8-D2ED-1057-3018-40E59C42A40D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -521,8 +539,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9775825" y="676273"/>
-          <a:ext cx="2778125" cy="3121027"/>
+          <a:off x="7759700" y="2419350"/>
+          <a:ext cx="2298700" cy="1587500"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -557,76 +575,122 @@
         <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-ES" sz="1100"/>
-            <a:t>connect by looking</a:t>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>so cool ideas</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>1) error</a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t> at which streams connect to the next intervall (i.e wat are the reactor inputs and how are they connected to their outputs)</a:t>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> mesaging while reading the excel</a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
           <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>0 -&gt; not connencted </a:t>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>2° could keep the interval names (in the code) as capital letters -&gt; no replace conflicts no more</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>1 -&gt; connected </a:t>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>3° write ALL eqation to the objects, read the equations there in steady of making it messy </a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
-        </a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>908050</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="CuadroTexto 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11D50F2C-E93D-46D5-95A9-E24286A73041}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7874000" y="635000"/>
+          <a:ext cx="2298700" cy="1587500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
         <a:p>
           <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>1's in the same colunm indiacte that the outputs of the intervals are mixed</a:t>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>compositions should be</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
-        </a:p>
-        <a:p>
           <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>string -&gt; defined how reject and permate are connected</a:t>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t> as followed </a:t>
           </a:r>
         </a:p>
         <a:p>
-          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+          <a:endParaRPr lang="en-GB" sz="1100" baseline="0"/>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>options :</a:t>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>components	compostion</a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>bool, permeat / reject </a:t>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>     glu, prot	   0.2, 0.8 </a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>split, permeate/ reject  </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
-            <a:t>mix permeate/ reject </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -636,6 +700,151 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>460375</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>123823</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>184150</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2166CD1C-89AD-4CD0-85A6-EA82146B47E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10702925" y="860423"/>
+          <a:ext cx="2778125" cy="4092577"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100"/>
+            <a:t>connect by looking</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t> at which streams connect to the next intervall (i.e wat are the reactor inputs and how are they connected to their outputs)</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>0 -&gt; not connencted </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>1 -&gt; connected </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>mix in the same colunm indiacte that the outputs of the intervals are mixed</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>sep_nr = define which seperation stream goes where</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>split_nr = define which split streqm goes where</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>options :</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>bool, split, sep 0 or  1</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="es-ES" sz="1100" baseline="0"/>
+            <a:t>can be a combination </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="es-ES" sz="1100" baseline="0"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1034,7 +1243,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1083,7 +1292,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C2">
         <v>20</v>
@@ -1106,10 +1315,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>64</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -1118,16 +1327,16 @@
         <v>100</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>0</v>
+      <c r="G3" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="H3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1135,7 +1344,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>0</v>
@@ -1161,7 +1370,7 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -1187,7 +1396,7 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1213,7 +1422,7 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1239,7 +1448,7 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -1262,10 +1471,10 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -1277,13 +1486,13 @@
         <v>0</v>
       </c>
       <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="13" t="s">
-        <v>45</v>
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1291,7 +1500,7 @@
         <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -1303,10 +1512,10 @@
         <v>0</v>
       </c>
       <c r="F10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -1317,7 +1526,7 @@
         <v>3</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C11">
         <v>0</v>
@@ -1329,26 +1538,51 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="H11">
         <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G12" s="13"/>
+      <c r="A12">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>100</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="E13:G13 E2:F11 H2:H11">
+  <conditionalFormatting sqref="E13:G13 E2:F2 E4:F12 E3 H2:H12">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1357,7 +1591,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1383,7 +1617,7 @@
         <v>11</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>35</v>
@@ -1398,13 +1632,13 @@
         <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="J1" s="16" t="s">
         <v>58</v>
-      </c>
-      <c r="J1" s="16" t="s">
-        <v>59</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>8</v>
@@ -1424,10 +1658,10 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" t="s">
         <v>51</v>
-      </c>
-      <c r="E2" t="s">
-        <v>52</v>
       </c>
       <c r="F2">
         <v>0.26675654674413302</v>
@@ -1439,7 +1673,7 @@
         <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J2" s="14" t="s">
         <v>60</v>
@@ -1462,10 +1696,10 @@
         <v>34</v>
       </c>
       <c r="D3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F3">
         <v>0.28253562825913597</v>
@@ -1477,7 +1711,7 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J3" s="14" t="s">
         <v>60</v>
@@ -1500,10 +1734,10 @@
         <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4">
         <v>0.26792861197630802</v>
@@ -1515,7 +1749,7 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J4" s="14" t="s">
         <v>60</v>
@@ -1538,10 +1772,10 @@
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5">
         <v>0.376575631424244</v>
@@ -1553,7 +1787,7 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J5" s="14" t="s">
         <v>60</v>
@@ -1576,10 +1810,10 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F6">
         <v>0.23511946945464801</v>
@@ -1591,7 +1825,7 @@
         <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J6" s="14" t="s">
         <v>60</v>
@@ -1611,28 +1845,28 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="F7" s="13">
         <v>0</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="K7">
         <v>0</v>
@@ -1653,10 +1887,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9730D4B9-BF36-445D-9853-EF3DA446843F}">
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1669,391 +1903,464 @@
     <col min="6" max="6" width="14.81640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.26953125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="9" max="9" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
     <col min="13" max="13" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J1" t="s">
         <v>47</v>
       </c>
-      <c r="C1" t="s">
+      <c r="K1" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="G2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0</v>
+      </c>
+      <c r="K2" s="1">
+        <v>0</v>
+      </c>
+      <c r="L2" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="B4" s="1">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K4" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="B6" s="1">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="11">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11">
+        <v>0</v>
+      </c>
+      <c r="I6" s="11">
+        <v>0</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K6" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B7" s="1">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
         <v>27</v>
       </c>
-      <c r="H1" t="s">
+      <c r="B8" s="1">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="L8" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J1" t="s">
-        <v>49</v>
-      </c>
-      <c r="K1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="1">
-        <v>0</v>
-      </c>
-      <c r="C2" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="F2" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="1">
-        <v>0</v>
-      </c>
-      <c r="J2" s="1">
-        <v>0</v>
-      </c>
-      <c r="K2" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1">
-        <v>0</v>
-      </c>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
-        <v>0</v>
-      </c>
-      <c r="E3" s="1">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0</v>
-      </c>
-      <c r="G3" s="1">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1">
-        <v>0</v>
-      </c>
-      <c r="I3" s="17" t="s">
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="J3" s="17" t="s">
+      <c r="L9" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="K3" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="1">
-        <v>0</v>
-      </c>
-      <c r="C4" s="1">
-        <v>0</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1">
-        <v>0</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K4" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1">
-        <v>0</v>
-      </c>
-      <c r="C5" s="1">
-        <v>0</v>
-      </c>
-      <c r="D5" s="1">
-        <v>0</v>
-      </c>
-      <c r="E5" s="1">
-        <v>0</v>
-      </c>
-      <c r="F5" s="11">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
-        <v>0</v>
-      </c>
-      <c r="H5" s="11">
-        <v>0</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J5" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="1">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>0</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J6" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="1"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" s="1">
-        <v>0</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J7" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>32</v>
-      </c>
-      <c r="B8" s="1">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <v>0</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
-        <v>0</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J8" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="K8" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="B10" s="1">
+        <v>0</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>0</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0</v>
+      </c>
+      <c r="I10" s="1">
+        <v>0</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0</v>
+      </c>
+      <c r="L10" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1">
-        <v>0</v>
-      </c>
-      <c r="C10" s="1">
-        <v>0</v>
-      </c>
-      <c r="D10" s="1">
-        <v>0</v>
-      </c>
-      <c r="E10" s="1">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1">
-        <v>0</v>
-      </c>
-      <c r="J10" s="1">
-        <v>0</v>
-      </c>
-      <c r="K10" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>0</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0</v>
+      </c>
+      <c r="I11" s="1">
+        <v>0</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0</v>
+      </c>
+      <c r="L11" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B11" s="1">
-        <v>0</v>
-      </c>
-      <c r="C11" s="1">
-        <v>0</v>
-      </c>
-      <c r="D11" s="1">
-        <v>0</v>
-      </c>
-      <c r="E11" s="1">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1">
-        <v>0</v>
-      </c>
-      <c r="I11" s="1">
-        <v>0</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="1">
+      <c r="B12" s="1">
+        <v>0</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
         <v>0</v>
       </c>
     </row>
@@ -2080,7 +2387,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:M13">
-    <cfRule type="colorScale" priority="1">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>

</xml_diff>